<commit_message>
2023/03/08 ebook 내서제 테이블 추가
</commit_message>
<xml_diff>
--- a/스토리보드/침대학교 테이블 v1.0.xlsx
+++ b/스토리보드/침대학교 테이블 v1.0.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\java1\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\java1\Desktop\Workspace\ChimAcademy\스토리보드\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15375" windowHeight="12195"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15375" windowHeight="12195" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="회원" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="수강" sheetId="6" r:id="rId4"/>
     <sheet name="학생" sheetId="3" r:id="rId5"/>
     <sheet name="교수" sheetId="5" r:id="rId6"/>
+    <sheet name="ebook" sheetId="7" r:id="rId7"/>
+    <sheet name="내서재" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="187">
   <si>
     <t>물리</t>
   </si>
@@ -577,6 +579,198 @@
   </si>
   <si>
     <t>state</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>테이블명 : cu_ebook</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>bookId</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>title</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>cate1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>cate2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>author</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>publisher</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>belong</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>loan</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>reserv</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>like</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>support</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>카테고리1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>카테고리2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>저자</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>출판사</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>소속도서관</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>대출</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>예약</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>대출 최대 5</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>예약 최대 5</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>책 제목</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>책 저자</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>책 출판사</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>좋아요</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>지원기기</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>VARCHAR(20)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>not null</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>not null</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>추천 기능</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC, mobilie,태블릿 등</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>group</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>그룹</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>주제별(인문,철학 등)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>그룹(전자책,구독형,오디오북)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>하위 카테고리(인문학,비문학 등)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>구홍모</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>cu_mylib</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>uid</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>bookId</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pubDate</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>출판일</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>책을 출판한 날짜</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>returnDate</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>loanDate</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>return</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1182,41 +1376,41 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1500,7 +1694,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
@@ -1842,24 +2036,24 @@
       <c r="H22" s="31"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="46" t="s">
+      <c r="B23" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="47" t="s">
+      <c r="C23" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="D23" s="48" t="s">
+      <c r="D23" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="E23" s="48"/>
-      <c r="F23" s="49" t="s">
+      <c r="E23" s="46"/>
+      <c r="F23" s="47" t="s">
         <v>129</v>
       </c>
-      <c r="G23" s="48"/>
-      <c r="H23" s="50"/>
+      <c r="G23" s="46"/>
+      <c r="H23" s="48"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B24" s="51" t="s">
+      <c r="B24" s="49" t="s">
         <v>119</v>
       </c>
       <c r="C24" s="21" t="s">
@@ -1876,7 +2070,7 @@
       <c r="H24" s="31"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B25" s="51" t="s">
+      <c r="B25" s="49" t="s">
         <v>120</v>
       </c>
       <c r="C25" s="21" t="s">
@@ -1893,7 +2087,7 @@
       <c r="H25" s="31"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="51" t="s">
+      <c r="B26" s="49" t="s">
         <v>84</v>
       </c>
       <c r="C26" s="21" t="s">
@@ -1910,10 +2104,10 @@
       <c r="H26" s="31"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="52" t="s">
+      <c r="B27" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="C27" s="53" t="s">
+      <c r="C27" s="51" t="s">
         <v>83</v>
       </c>
       <c r="D27" s="34" t="s">
@@ -1950,10 +2144,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="52" t="s">
         <v>108</v>
       </c>
-      <c r="C1" s="42"/>
+      <c r="C1" s="53"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
@@ -2107,7 +2301,7 @@
       <c r="D12" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="45" t="s">
+      <c r="F12" s="43" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2121,7 +2315,7 @@
       <c r="D13" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="45" t="s">
+      <c r="F13" s="43" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2368,10 +2562,10 @@
       <c r="B14" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="C14" s="44" t="s">
+      <c r="C14" s="42" t="s">
         <v>117</v>
       </c>
-      <c r="D14" s="44" t="s">
+      <c r="D14" s="42" t="s">
         <v>47</v>
       </c>
       <c r="F14" s="25" t="s">
@@ -2856,7 +3050,7 @@
   <dimension ref="B1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3023,4 +3217,477 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:H18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="13.25" customWidth="1"/>
+    <col min="5" max="5" width="20.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B6" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="10"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="G7" s="14"/>
+      <c r="H7" s="15"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B8" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="G8" s="14"/>
+      <c r="H8" s="15"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="G9" s="14"/>
+      <c r="H9" s="15"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B10" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="G10" s="14"/>
+      <c r="H10" s="15"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B11" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="G11" s="14"/>
+      <c r="H11" s="15"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B12" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="G12" s="14"/>
+      <c r="H12" s="15"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B13" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="13"/>
+      <c r="F13" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="G13" s="14"/>
+      <c r="H13" s="15"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B14" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="F14" s="11">
+        <v>0</v>
+      </c>
+      <c r="G14" s="14"/>
+      <c r="H14" s="15"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B15" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="F15" s="11">
+        <v>0</v>
+      </c>
+      <c r="G15" s="14"/>
+      <c r="H15" s="15"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B16" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="F16" s="11">
+        <v>0</v>
+      </c>
+      <c r="G16" s="14"/>
+      <c r="H16" s="15"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B17" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="G17" s="14"/>
+      <c r="H17" s="15"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B18" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="G18" s="14"/>
+      <c r="H18" s="15"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:H17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B6" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="10"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="C7" s="12"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="15"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B8" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="C8" s="12"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="15"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="15"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B10" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="15"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B11" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="15"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B12" s="16"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="15"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B13" s="16"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="15"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B14" s="16"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="15"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B15" s="16"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="15"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B16" s="16"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="15"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B17" s="16"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="15"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>